<commit_message>
Stable Version for ShippingTable
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -63,18 +63,12 @@
     <t>Intent</t>
   </si>
   <si>
-    <t>This is test</t>
-  </si>
-  <si>
     <t>Proactiv</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>Catalog</t>
-  </si>
-  <si>
     <t>Meaningful Beauty</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>03/16/2016</t>
-  </si>
-  <si>
     <t>StartDate (mm/dd/yyyy)</t>
   </si>
   <si>
@@ -108,23 +99,25 @@
     <t>ShippingTableCode</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>No of ShippingRange</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>Catalog Offers</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>S37B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,22 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill>
-        <bgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
+      <patternFill patternType="none">
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -174,13 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,30 +497,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,22 +549,19 @@
         <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -602,32 +574,23 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="N2" t="s" s="5">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -660,10 +623,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -682,38 +645,38 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -731,10 +694,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>